<commit_message>
adding a2a tests from Brad
</commit_message>
<xml_diff>
--- a/Command Coverage.xlsx
+++ b/Command Coverage.xlsx
@@ -1408,12 +1408,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H354"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="6" topLeftCell="A334" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="6" topLeftCell="A259" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E344" activeCellId="0" sqref="E344"/>
+      <selection pane="bottomLeft" activeCell="D272" activeCellId="0" sqref="D272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.3359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1444,11 +1444,11 @@
       </c>
       <c r="B2" s="1" t="n">
         <f aca="false">COUNTIF(C7:C354,"Yes")</f>
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="C2" s="2" t="n">
         <f aca="false">B2/B1</f>
-        <v>0.804597701149425</v>
+        <v>0.844827586206896</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1457,11 +1457,11 @@
       </c>
       <c r="B3" s="1" t="n">
         <f aca="false">COUNTIF(D7:D354,"Yes")</f>
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2" t="n">
         <f aca="false">B3/B1</f>
-        <v>0.195402298850575</v>
+        <v>0.155172413793103</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1511,7 +1511,7 @@
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -3047,7 +3047,7 @@
       <c r="B80" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E80" s="1" t="s">
@@ -3068,7 +3068,7 @@
       <c r="B81" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E81" s="1" t="s">
@@ -3089,7 +3089,7 @@
       <c r="B82" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="C82" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E82" s="1" t="s">
@@ -3110,7 +3110,7 @@
       <c r="B83" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E83" s="1" t="s">
@@ -3131,7 +3131,7 @@
       <c r="B84" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E84" s="1" t="s">
@@ -3152,7 +3152,7 @@
       <c r="B85" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="C85" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E85" s="1" t="s">
@@ -3173,7 +3173,7 @@
       <c r="B86" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D86" s="1" t="s">
+      <c r="C86" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E86" s="1" t="s">
@@ -3194,7 +3194,7 @@
       <c r="B87" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="C87" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E87" s="1" t="s">
@@ -6345,7 +6345,7 @@
       <c r="B236" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D236" s="1" t="s">
+      <c r="C236" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E236" s="1" t="s">
@@ -7101,7 +7101,7 @@
       <c r="B272" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D272" s="1" t="s">
+      <c r="C272" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E272" s="1" t="s">
@@ -7884,7 +7884,7 @@
       <c r="B309" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D309" s="1" t="s">
+      <c r="C309" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E309" s="1" t="s">
@@ -7905,7 +7905,7 @@
       <c r="B310" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D310" s="1" t="s">
+      <c r="C310" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E310" s="1" t="s">
@@ -8034,7 +8034,7 @@
       <c r="B316" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D316" s="1" t="s">
+      <c r="C316" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E316" s="1" t="s">
@@ -8848,6 +8848,8 @@
         <v>Wait</v>
       </c>
     </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A6:H354">
     <sortState ref="A7:H354">
@@ -9233,13 +9235,13 @@
         <f aca="false">IF(ISNA(VLOOKUP(A14,'Command List v6 LTS'!$A$6:$A$354,1,FALSE())),"Yes","")</f>
         <v/>
       </c>
-      <c r="J14" s="6" t="n">
+      <c r="J14" s="6" t="str">
         <f aca="false">IF(I14="",VLOOKUP(A14,'Command List v6 LTS'!$A$7:$D$354,3,FALSE()),C14)</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
       <c r="K14" s="6" t="str">
         <f aca="false">IF(I14="",IF(J14="Yes","",VLOOKUP(A14,'Command List v6 LTS'!$A$7:$D$354,4,FALSE())),"")</f>
-        <v>Yes</v>
+        <v/>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11709,13 +11711,13 @@
         <f aca="false">IF(ISNA(VLOOKUP(A87,'Command List v6 LTS'!$A$6:$A$354,1,FALSE())),"Yes","")</f>
         <v/>
       </c>
-      <c r="J87" s="6" t="n">
+      <c r="J87" s="6" t="str">
         <f aca="false">IF(I87="",VLOOKUP(A87,'Command List v6 LTS'!$A$7:$D$354,3,FALSE()),C87)</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
       <c r="K87" s="6" t="str">
         <f aca="false">IF(I87="",IF(J87="Yes","",VLOOKUP(A87,'Command List v6 LTS'!$A$7:$D$354,4,FALSE())),"")</f>
-        <v>Yes</v>
+        <v/>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11743,13 +11745,13 @@
         <f aca="false">IF(ISNA(VLOOKUP(A88,'Command List v6 LTS'!$A$6:$A$354,1,FALSE())),"Yes","")</f>
         <v/>
       </c>
-      <c r="J88" s="6" t="n">
+      <c r="J88" s="6" t="str">
         <f aca="false">IF(I88="",VLOOKUP(A88,'Command List v6 LTS'!$A$7:$D$354,3,FALSE()),C88)</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
       <c r="K88" s="6" t="str">
         <f aca="false">IF(I88="",IF(J88="Yes","",VLOOKUP(A88,'Command List v6 LTS'!$A$7:$D$354,4,FALSE())),"")</f>
-        <v>Yes</v>
+        <v/>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11777,13 +11779,13 @@
         <f aca="false">IF(ISNA(VLOOKUP(A89,'Command List v6 LTS'!$A$6:$A$354,1,FALSE())),"Yes","")</f>
         <v/>
       </c>
-      <c r="J89" s="6" t="n">
+      <c r="J89" s="6" t="str">
         <f aca="false">IF(I89="",VLOOKUP(A89,'Command List v6 LTS'!$A$7:$D$354,3,FALSE()),C89)</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
       <c r="K89" s="6" t="str">
         <f aca="false">IF(I89="",IF(J89="Yes","",VLOOKUP(A89,'Command List v6 LTS'!$A$7:$D$354,4,FALSE())),"")</f>
-        <v>Yes</v>
+        <v/>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11811,13 +11813,13 @@
         <f aca="false">IF(ISNA(VLOOKUP(A90,'Command List v6 LTS'!$A$6:$A$354,1,FALSE())),"Yes","")</f>
         <v/>
       </c>
-      <c r="J90" s="6" t="n">
+      <c r="J90" s="6" t="str">
         <f aca="false">IF(I90="",VLOOKUP(A90,'Command List v6 LTS'!$A$7:$D$354,3,FALSE()),C90)</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
       <c r="K90" s="6" t="str">
         <f aca="false">IF(I90="",IF(J90="Yes","",VLOOKUP(A90,'Command List v6 LTS'!$A$7:$D$354,4,FALSE())),"")</f>
-        <v>Yes</v>
+        <v/>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11845,13 +11847,13 @@
         <f aca="false">IF(ISNA(VLOOKUP(A91,'Command List v6 LTS'!$A$6:$A$354,1,FALSE())),"Yes","")</f>
         <v/>
       </c>
-      <c r="J91" s="6" t="n">
+      <c r="J91" s="6" t="str">
         <f aca="false">IF(I91="",VLOOKUP(A91,'Command List v6 LTS'!$A$7:$D$354,3,FALSE()),C91)</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
       <c r="K91" s="6" t="str">
         <f aca="false">IF(I91="",IF(J91="Yes","",VLOOKUP(A91,'Command List v6 LTS'!$A$7:$D$354,4,FALSE())),"")</f>
-        <v>Yes</v>
+        <v/>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11879,13 +11881,13 @@
         <f aca="false">IF(ISNA(VLOOKUP(A92,'Command List v6 LTS'!$A$6:$A$354,1,FALSE())),"Yes","")</f>
         <v/>
       </c>
-      <c r="J92" s="6" t="n">
+      <c r="J92" s="6" t="str">
         <f aca="false">IF(I92="",VLOOKUP(A92,'Command List v6 LTS'!$A$7:$D$354,3,FALSE()),C92)</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
       <c r="K92" s="6" t="str">
         <f aca="false">IF(I92="",IF(J92="Yes","",VLOOKUP(A92,'Command List v6 LTS'!$A$7:$D$354,4,FALSE())),"")</f>
-        <v>Yes</v>
+        <v/>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11913,13 +11915,13 @@
         <f aca="false">IF(ISNA(VLOOKUP(A93,'Command List v6 LTS'!$A$6:$A$354,1,FALSE())),"Yes","")</f>
         <v/>
       </c>
-      <c r="J93" s="6" t="n">
+      <c r="J93" s="6" t="str">
         <f aca="false">IF(I93="",VLOOKUP(A93,'Command List v6 LTS'!$A$7:$D$354,3,FALSE()),C93)</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
       <c r="K93" s="6" t="str">
         <f aca="false">IF(I93="",IF(J93="Yes","",VLOOKUP(A93,'Command List v6 LTS'!$A$7:$D$354,4,FALSE())),"")</f>
-        <v>Yes</v>
+        <v/>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11947,13 +11949,13 @@
         <f aca="false">IF(ISNA(VLOOKUP(A94,'Command List v6 LTS'!$A$6:$A$354,1,FALSE())),"Yes","")</f>
         <v/>
       </c>
-      <c r="J94" s="6" t="n">
+      <c r="J94" s="6" t="str">
         <f aca="false">IF(I94="",VLOOKUP(A94,'Command List v6 LTS'!$A$7:$D$354,3,FALSE()),C94)</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
       <c r="K94" s="6" t="str">
         <f aca="false">IF(I94="",IF(J94="Yes","",VLOOKUP(A94,'Command List v6 LTS'!$A$7:$D$354,4,FALSE())),"")</f>
-        <v>Yes</v>
+        <v/>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17019,13 +17021,13 @@
         <f aca="false">IF(ISNA(VLOOKUP(A243,'Command List v6 LTS'!$A$6:$A$354,1,FALSE())),"Yes","")</f>
         <v/>
       </c>
-      <c r="J243" s="6" t="n">
+      <c r="J243" s="6" t="str">
         <f aca="false">IF(I243="",VLOOKUP(A243,'Command List v6 LTS'!$A$7:$D$354,3,FALSE()),C243)</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
       <c r="K243" s="6" t="str">
         <f aca="false">IF(I243="",IF(J243="Yes","",VLOOKUP(A243,'Command List v6 LTS'!$A$7:$D$354,4,FALSE())),"")</f>
-        <v>Yes</v>
+        <v/>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18201,13 +18203,13 @@
         <f aca="false">IF(ISNA(VLOOKUP(A278,'Command List v6 LTS'!$A$6:$A$354,1,FALSE())),"Yes","")</f>
         <v/>
       </c>
-      <c r="J278" s="6" t="n">
+      <c r="J278" s="6" t="str">
         <f aca="false">IF(I278="",VLOOKUP(A278,'Command List v6 LTS'!$A$7:$D$354,3,FALSE()),C278)</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
       <c r="K278" s="6" t="str">
         <f aca="false">IF(I278="",IF(J278="Yes","",VLOOKUP(A278,'Command List v6 LTS'!$A$7:$D$354,4,FALSE())),"")</f>
-        <v>Yes</v>
+        <v/>
       </c>
     </row>
     <row r="279" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19427,13 +19429,13 @@
         <f aca="false">IF(ISNA(VLOOKUP(A314,'Command List v6 LTS'!$A$6:$A$354,1,FALSE())),"Yes","")</f>
         <v/>
       </c>
-      <c r="J314" s="6" t="n">
+      <c r="J314" s="6" t="str">
         <f aca="false">IF(I314="",VLOOKUP(A314,'Command List v6 LTS'!$A$7:$D$354,3,FALSE()),C314)</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
       <c r="K314" s="6" t="str">
         <f aca="false">IF(I314="",IF(J314="Yes","",VLOOKUP(A314,'Command List v6 LTS'!$A$7:$D$354,4,FALSE())),"")</f>
-        <v>Yes</v>
+        <v/>
       </c>
     </row>
     <row r="315" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19461,13 +19463,13 @@
         <f aca="false">IF(ISNA(VLOOKUP(A315,'Command List v6 LTS'!$A$6:$A$354,1,FALSE())),"Yes","")</f>
         <v/>
       </c>
-      <c r="J315" s="6" t="n">
+      <c r="J315" s="6" t="str">
         <f aca="false">IF(I315="",VLOOKUP(A315,'Command List v6 LTS'!$A$7:$D$354,3,FALSE()),C315)</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
       <c r="K315" s="6" t="str">
         <f aca="false">IF(I315="",IF(J315="Yes","",VLOOKUP(A315,'Command List v6 LTS'!$A$7:$D$354,4,FALSE())),"")</f>
-        <v>Yes</v>
+        <v/>
       </c>
     </row>
     <row r="316" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19633,13 +19635,13 @@
         <f aca="false">IF(ISNA(VLOOKUP(A320,'Command List v6 LTS'!$A$6:$A$354,1,FALSE())),"Yes","")</f>
         <v/>
       </c>
-      <c r="J320" s="6" t="n">
+      <c r="J320" s="6" t="str">
         <f aca="false">IF(I320="",VLOOKUP(A320,'Command List v6 LTS'!$A$7:$D$354,3,FALSE()),C320)</f>
-        <v>0</v>
+        <v>Yes</v>
       </c>
       <c r="K320" s="6" t="str">
         <f aca="false">IF(I320="",IF(J320="Yes","",VLOOKUP(A320,'Command List v6 LTS'!$A$7:$D$354,4,FALSE())),"")</f>
-        <v>Yes</v>
+        <v/>
       </c>
     </row>
     <row r="321" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>